<commit_message>
more data in consumers
</commit_message>
<xml_diff>
--- a/documents/kumbio_modelo datos 25-10.xlsx
+++ b/documents/kumbio_modelo datos 25-10.xlsx
@@ -857,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -882,7 +882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -907,7 +907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -932,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -957,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -982,7 +982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1199,7 +1199,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1250,7 +1250,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>

</xml_diff>